<commit_message>
The busiest day in Caltrans, 8 Gantt Charts.
try to use access to combine history and scenario data and lookup budget
group for history data. add more lookup fields to the pivot chart
template.
</commit_message>
<xml_diff>
--- a/for Hector/Tom/Good Data/SF001LEFT-Done.xlsx
+++ b/for Hector/Tom/Good Data/SF001LEFT-Done.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shq153\Desktop\Caltrans\for Hector\Tom\Good Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535"/>
   </bookViews>
@@ -309,6 +314,9 @@
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -335,6 +343,9 @@
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -361,6 +372,9 @@
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -387,6 +401,9 @@
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -404,6 +421,9 @@
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>Grind/Replace slabs - 04-107CBT - Beg PM:    6.330 - End PM:7.077 - CAPM, Length: 0.747</a:t>
@@ -411,12 +431,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:spPr/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -434,6 +460,9 @@
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>HMA Medium Overlay - 04-4C130 - Beg PM:    0.000 - End PM: 6.330 - CAPM, Length: 6.33</a:t>
@@ -441,12 +470,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:spPr/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -464,6 +499,9 @@
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>HMA Thick Overlay - 04-23290 - Beg PM:    0.336 - End PM: 1.600 - Rehab, Length: 1.264</a:t>
@@ -471,12 +509,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:spPr/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -494,6 +538,9 @@
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>HMA Medium Overlay - 04-23290 - Beg PM:    2.100 - End PM: 4.100 - Rehab, Length: 2</a:t>
@@ -501,12 +548,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:spPr/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="1"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -612,6 +665,11 @@
               <c:showSerName val="1"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:spPr/>
             <c:txPr>
@@ -631,6 +689,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -704,6 +767,11 @@
               <c:showSerName val="1"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:spPr/>
             <c:txPr>
@@ -723,6 +791,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -796,6 +869,11 @@
               <c:showSerName val="1"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:spPr/>
             <c:txPr>
@@ -815,6 +893,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -936,6 +1019,11 @@
               <c:showSerName val="1"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:spPr/>
             <c:txPr>
@@ -955,6 +1043,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -996,20 +1089,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="539011072"/>
-        <c:axId val="502584960"/>
+        <c:axId val="178640128"/>
+        <c:axId val="178640512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539011072"/>
+        <c:axId val="178640128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="502584960"/>
+        <c:crossAx val="178640512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1017,7 +1111,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="502584960"/>
+        <c:axId val="178640512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539011072"/>
+        <c:crossAx val="178640128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2038,7 +2132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>